<commit_message>
Update examples to always have an id column
</commit_message>
<xml_diff>
--- a/examples/demo-pregnancy-cases.xlsx
+++ b/examples/demo-pregnancy-cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="860" windowWidth="21520" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pregnant Mother Cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Data Source</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>`this`</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>`this`</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In order to sync with a SQL database, id is mandatory</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -126,12 +138,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -513,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -604,12 +610,12 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://openrosa.org/formdesigner/dd3190c7dd7e9e7d469a9705709f2f6b4e27f1d8"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -620,19 +626,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -667,7 +674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="E3" t="s">
         <v>23</v>
       </c>
@@ -675,13 +682,24 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://openrosa.org/formdesigner/dd3190c7dd7e9e7d469a9705709f2f6b4e27f1d8"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>